<commit_message>
Built site for MassWateR: 1.0.0.9000@baf7667
</commit_message>
<xml_diff>
--- a/MassWateR_DQOAccuracy_Template.xlsx
+++ b/MassWateR_DQOAccuracy_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2FCA00-22D3-4804-A1EC-B988BA0E6C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2F4364-55A3-4566-8946-43A2797B5628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
     <t>The range of results values that the data quality objectives will apply to.  Create one row for each range and list them in order of lowest to highest.  Enter "all" if no ranges are specified.  For formatting, it doesn't matter whether there are spaces between the characters or not.  See below for an example of how ranges work.</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter the spike or calibration check data quality objective.  This will be used for Lab Spikes and Instrument Calibration Checks.  </t>
+    <t>Enter the spike or calibration check data quality objective.  This will be used for Lab Spikes and Instrument Calibration Checks.  This can also be used for performance evaluation samples, such as outside standards that are used to assess lab analytical accuracy.</t>
   </si>
 </sst>
 </file>
@@ -341,23 +341,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -400,6 +390,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,338 +792,338 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973C1027-43ED-409D-9786-38F45BEFD8D3}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="10" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="5" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="5" customWidth="1"/>
+    <col min="5" max="10" width="12.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="18">
         <v>0.1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="18">
         <v>0.1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="18">
         <v>0.01</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="18" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="18">
         <v>0.01</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="18">
         <v>10</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="18">
         <v>2400</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="18">
         <v>10</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="18">
         <v>2400</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="18">
         <v>10</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="18">
         <v>2400</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="18">
         <v>10</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="18">
         <v>2400</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1132,11 +1137,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83CEA30-4E88-458A-AFF2-D4098CA8390C}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,184 +1153,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="13">
         <v>0.1</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>1500</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="17" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Built site for MassWateR: 2.1.1@d4cc0e8
</commit_message>
<xml_diff>
--- a/MassWateR_DQOAccuracy_Template.xlsx
+++ b/MassWateR_DQOAccuracy_Template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65957BB8-1042-4E40-8C0C-E7F22CBA5A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8557988E-4E29-4824-A2B2-C842145FABF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
     <sheet name="Instructions" sheetId="2" r:id="rId2"/>
+    <sheet name="Values" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="164">
   <si>
     <t>Parameter</t>
   </si>
@@ -190,9 +191,6 @@
     <t>Result unit of measure.  Only the units of measure listed in the parameter list are allowed.</t>
   </si>
   <si>
-    <t>Minimum Detection Level.  If the Result Value is BDL and no value is entered in the Results file Quantitation Limit column, then this value will be used.  MassWateR analytical functions will use 1/2 of the MDL for data purposes.</t>
-  </si>
-  <si>
     <t>&lt;, &lt;=, &gt;, &gt;=, log, %, BDL, na</t>
   </si>
   <si>
@@ -217,9 +215,6 @@
     <t>All cells in the matrix must either have a value or "na".</t>
   </si>
   <si>
-    <t>Upper Quantitation Limit.  If the Result Value is AQL and no value is entered in the Results file Quantitation Limit column, then this value will be used.  MassWateR analytical functions will use 100% of the UQL for data purposes.</t>
-  </si>
-  <si>
     <t>numeric, or na</t>
   </si>
   <si>
@@ -232,7 +227,307 @@
     <t>Enter the spike or calibration check data quality objective.  This will be used for Lab Spikes and Instrument Calibration Checks.  This can also be used for performance evaluation samples, such as outside standards that are used to assess lab analytical accuracy.</t>
   </si>
   <si>
-    <t>Template updated 12/7/22</t>
+    <t>Upper Quantitation Limit.  If the Result Value is AQL and no value is entered in the Results file Quantitation Limit column, then this value will be used.  Enter "na" if there is no limit.  MassWateR analytical functions will use 100% of the UQL for data purposes.</t>
+  </si>
+  <si>
+    <t>Template updated 8/16/23</t>
+  </si>
+  <si>
+    <t>Minimum Detection Level.  If the Result Value is BDL and no value is entered in the Results file Quantitation Limit column, then this value will be used.  Enter "na" if there is no minimum.  MassWateR analytical functions will use 1/2 of the MDL for data purposes.</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>Air Temp</t>
+  </si>
+  <si>
+    <t>#/100ml</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Algae, blue-green (phylum cyanophyta) density</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>% recovery</t>
+  </si>
+  <si>
+    <t>Ammonium</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>Chl a</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>Chl a (probe)</t>
+  </si>
+  <si>
+    <t>cfm</t>
+  </si>
+  <si>
+    <t>Chloride</t>
+  </si>
+  <si>
+    <t>cfs</t>
+  </si>
+  <si>
+    <t>Chlorophyll a</t>
+  </si>
+  <si>
+    <t>Chlorophyll a (probe)</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Chlorophyll a (probe) concentration, Cyanobacteria (bluegreen)</t>
+  </si>
+  <si>
+    <t>deg C</t>
+  </si>
+  <si>
+    <t>Conductivity</t>
+  </si>
+  <si>
+    <t>deg F</t>
+  </si>
+  <si>
+    <t>Cyanobacteria (lab)</t>
+  </si>
+  <si>
+    <t>FAU</t>
+  </si>
+  <si>
+    <t>Cyanobacteria (probe)</t>
+  </si>
+  <si>
+    <t>FBU</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>FNMU</t>
+  </si>
+  <si>
+    <t>Depth, Secchi disk depth</t>
+  </si>
+  <si>
+    <t>FNRU</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen (DO)</t>
+  </si>
+  <si>
+    <t>FNU</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen saturation</t>
+  </si>
+  <si>
+    <t>FTU</t>
+  </si>
+  <si>
+    <t>DO saturation</t>
+  </si>
+  <si>
+    <t>g/kg</t>
+  </si>
+  <si>
+    <t>JTU</t>
+  </si>
+  <si>
+    <t>Enterococcus</t>
+  </si>
+  <si>
+    <t>l/min</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>l/sec</t>
+  </si>
+  <si>
+    <t>Fecal Coliform</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Gage</t>
+  </si>
+  <si>
+    <t>mgd</t>
+  </si>
+  <si>
+    <t>Height, gage</t>
+  </si>
+  <si>
+    <t>MPN/100ml</t>
+  </si>
+  <si>
+    <t>Metals</t>
+  </si>
+  <si>
+    <t>mS/cm</t>
+  </si>
+  <si>
+    <t>Microcystins</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>NTMU</t>
+  </si>
+  <si>
+    <t>Nitrate + Nitrite</t>
+  </si>
+  <si>
+    <t>NTRU</t>
+  </si>
+  <si>
+    <t>Nitrite</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>Ortho P</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>Orthophosphate</t>
+  </si>
+  <si>
+    <t>ppt</t>
+  </si>
+  <si>
+    <t>Particulate organic carbon</t>
+  </si>
+  <si>
+    <t>ppth</t>
+  </si>
+  <si>
+    <t>PSS</t>
+  </si>
+  <si>
+    <t>Pheophytin</t>
+  </si>
+  <si>
+    <t>PSU</t>
+  </si>
+  <si>
+    <t>Pheophytin a</t>
+  </si>
+  <si>
+    <t>Phosphorus, Particulate Organic</t>
+  </si>
+  <si>
+    <t>S/m</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>ug/l</t>
+  </si>
+  <si>
+    <t>PON</t>
+  </si>
+  <si>
+    <t>umol/l</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>uS/cm</t>
+  </si>
+  <si>
+    <t>Salinity</t>
+  </si>
+  <si>
+    <t>Secchi Depth</t>
+  </si>
+  <si>
+    <t>Silicate</t>
+  </si>
+  <si>
+    <t>Sp Conductance</t>
+  </si>
+  <si>
+    <t>Specific conductance</t>
+  </si>
+  <si>
+    <t>Sulfate</t>
+  </si>
+  <si>
+    <t>Surfactants</t>
+  </si>
+  <si>
+    <t>TDN</t>
+  </si>
+  <si>
+    <t>TDP</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>Temperature, air</t>
+  </si>
+  <si>
+    <t>Temperature, water</t>
+  </si>
+  <si>
+    <t>TKN</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>Total dissolved solids</t>
+  </si>
+  <si>
+    <t>Total Kjeldahl nitrogen</t>
+  </si>
+  <si>
+    <t>Total Nitrogen, mixed forms</t>
+  </si>
+  <si>
+    <t>Total Phosphorus, mixed forms</t>
+  </si>
+  <si>
+    <t>Total suspended solids</t>
+  </si>
+  <si>
+    <t>TSS</t>
+  </si>
+  <si>
+    <t>Turbidity</t>
+  </si>
+  <si>
+    <t>Water Temp</t>
   </si>
 </sst>
 </file>
@@ -282,7 +577,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +587,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -410,6 +711,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,7 +1108,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,6 +1442,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A4EA15E2-D832-4A49-BBD2-136FE3197BAC}">
+          <x14:formula1>
+            <xm:f>Values!$A$2:$A$65</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E51C4DBB-7A06-4B01-9EB2-015D10941B0A}">
+          <x14:formula1>
+            <xm:f>Values!$B$2:$B$42</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1146,7 +1471,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1487,7 @@
         <v>48</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1172,7 +1497,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1222,13 +1547,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C8" s="13">
         <v>0.1</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1236,13 +1561,13 @@
         <v>23</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C9" s="12">
         <v>1500</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1250,19 +1575,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1272,13 +1597,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,13 +1611,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,13 +1625,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,13 +1639,13 @@
         <v>21</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1328,18 +1653,18 @@
         <v>4</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1347,4 +1672,476 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618763B1-9045-410C-ABE3-5B174AA86A7D}">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>